<commit_message>
modif taille images dans css
</commit_message>
<xml_diff>
--- a/audit_la_chouette_agence.xlsx
+++ b/audit_la_chouette_agence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clement/Documents/formation/Projets/p4_vermeulen_clement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clement/Documents/formation/Projets/P4_vermeulen_clement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B41FEB1-C047-994D-A72F-5594774A9502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF0B32-35D0-F343-A4C8-C56469B9AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="760" windowWidth="29300" windowHeight="17200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>Catégorie</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Structure des titres incorrecte</t>
   </si>
   <si>
-    <t xml:space="preserve">Hiérarchie des titres non respectée </t>
-  </si>
-  <si>
     <t>Respecter l'ordre des balises h1,h2,…</t>
   </si>
   <si>
@@ -172,6 +169,15 @@
   </si>
   <si>
     <t>Ne pa utiliser d'image pour afficher du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiérarchie des balises titres non respectée </t>
+  </si>
+  <si>
+    <t>Modifier la couleur de police / agrandir la taille de police</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site#/id/r-6055853</t>
   </si>
 </sst>
 </file>
@@ -210,7 +216,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,12 +227,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -270,22 +270,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -506,7 +506,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -560,8 +560,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>21</v>
+      <c r="A2" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
@@ -569,18 +569,20 @@
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="6"/>
+      <c r="D2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>21</v>
+      <c r="A3" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>9</v>
@@ -588,11 +590,11 @@
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -600,8 +602,8 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>21</v>
+      <c r="A4" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
@@ -609,11 +611,11 @@
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>46</v>
+      <c r="D4" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -621,20 +623,20 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>27</v>
+      <c r="E5" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="4"/>
@@ -642,20 +644,20 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>21</v>
+      <c r="A6" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -663,20 +665,20 @@
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>21</v>
+      <c r="A7" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -684,7 +686,7 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -693,32 +695,34 @@
       <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>26</v>
+      <c r="D8" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -726,39 +730,39 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -777,7 +781,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="9"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Suppression de fichiers inutils
</commit_message>
<xml_diff>
--- a/audit_la_chouette_agence.xlsx
+++ b/audit_la_chouette_agence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clement/Documents/formation/Projets/P4_vermeulen_clement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF0B32-35D0-F343-A4C8-C56469B9AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C7A2C9-8361-AE46-8D8D-8809A6F9D102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Catégorie</t>
   </si>
@@ -177,14 +177,32 @@
     <t>Modifier la couleur de police / agrandir la taille de police</t>
   </si>
   <si>
-    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site#/id/r-6055853</t>
+    <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist#colour</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist#les_équivalents_textuels</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site#/id/r-6055853            https://www.seonity.com/format-image-webp-seo/</t>
+  </si>
+  <si>
+    <t>https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578346-augmentez-lautorite-de-votre-site#/id/r-5603088</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist#directives_générales</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/HTTP/Headers/Content-Language#indiquer_la_langue_dans_laquelle_un_document_est_%C3%A9crit%C2%A0liste%20des%20langues</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,6 +232,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -246,10 +270,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -285,11 +310,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,7 +535,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -515,7 +544,7 @@
     <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1"/>
     <col min="7" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -575,12 +604,14 @@
       <c r="E2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
@@ -596,7 +627,9 @@
       <c r="E3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -617,12 +650,14 @@
       <c r="E4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>20</v>
       </c>
@@ -638,7 +673,9 @@
       <c r="E5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -659,12 +696,14 @@
       <c r="E6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
@@ -680,12 +719,14 @@
       <c r="E7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
@@ -701,8 +742,8 @@
       <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>48</v>
+      <c r="F8" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -724,12 +765,14 @@
       <c r="E9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
@@ -745,10 +788,12 @@
       <c r="E10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>6</v>
       </c>
@@ -764,7 +809,9 @@
       <c r="E11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1833,6 +1880,10 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" location="les_équivalents_textuels" xr:uid="{BA495ABD-4592-AA4E-9CCA-1E966F57F1D7}"/>
+    <hyperlink ref="F8" r:id="rId2" location="/id/r-6055853" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site#/id/r-6055853" xr:uid="{D2C15B93-EFD9-7D41-B0D6-8C85A716877E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>